<commit_message>
Include URL fetching in Rule manager
</commit_message>
<xml_diff>
--- a/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
+++ b/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Issue Tracker" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Issue Tracker'!$A$1:$G$29</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="42">
   <si>
     <t>S.N</t>
   </si>
@@ -125,9 +128,6 @@
     <t>Store Proc to check and Update/Insert in Rule Engine table</t>
   </si>
   <si>
-    <t>Tool tip for Dashboard</t>
-  </si>
-  <si>
     <t>Web scraping(HTML Agility Pack): Parallal option for reading data from website in place of file upload. May be a radio button(From file/ From Website)</t>
   </si>
   <si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>New Page for Validation rule/ we can integrate it in Rule builder page (Need to decide)</t>
+  </si>
+  <si>
+    <t>Stop showing '0' with Running status in summary report</t>
+  </si>
+  <si>
+    <t>Tool tip for Dashboard menu</t>
+  </si>
+  <si>
+    <t>Show / Hide fileupload and url provider textbox in document provider radio button.</t>
   </si>
 </sst>
 </file>
@@ -519,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +887,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="11">
         <v>43166</v>
@@ -920,7 +929,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C17" s="11">
         <v>43166</v>
@@ -941,7 +950,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="11">
         <v>43166</v>
@@ -962,7 +971,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="11">
         <v>43166</v>
@@ -983,7 +992,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="11">
         <v>43166</v>
@@ -1004,7 +1013,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="11">
         <v>43166</v>
@@ -1021,26 +1030,48 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="B22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="7">
+        <v>43167</v>
+      </c>
+      <c r="D22" s="7">
+        <v>43167</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="B23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="11">
+        <v>43167</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -1109,6 +1140,7 @@
       <c r="G29" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G29"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>$U$2:$U$4</formula1>

</xml_diff>

<commit_message>
Web scrapping, design rectification
</commit_message>
<xml_diff>
--- a/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
+++ b/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
   <si>
     <t>S.N</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Implement http://www.redmine.org for issue tracking</t>
+  </si>
+  <si>
+    <t>Modal Popup containing null in time of web scrapping implementation</t>
+  </si>
+  <si>
+    <t>New Implementation</t>
   </si>
 </sst>
 </file>
@@ -553,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,26 +1000,28 @@
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="11">
-        <v>43166</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="C18" s="7">
+        <v>43166</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43171</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
@@ -1032,7 +1043,9 @@
       <c r="G19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -1125,28 +1138,48 @@
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="B24" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="11">
+        <v>43171</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="B25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="11">
+        <v>43171</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">

</xml_diff>

<commit_message>
Web scrapping, design rectification, other issue solving
</commit_message>
<xml_diff>
--- a/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
+++ b/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
   <si>
     <t>S.N</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>New Implementation</t>
+  </si>
+  <si>
+    <t>Valid Run ID message in Report Page while click on "0" RunID.</t>
   </si>
 </sst>
 </file>
@@ -562,14 +565,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -975,29 +978,33 @@
       <c r="G16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="11">
-        <v>43166</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="9" t="s">
+      <c r="C17" s="7">
+        <v>43166</v>
+      </c>
+      <c r="D17" s="7">
+        <v>43172</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="9"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
@@ -1021,7 +1028,9 @@
       <c r="G18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
@@ -1182,16 +1191,26 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="B26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="11">
+        <v>43171</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">

</xml_diff>

<commit_message>
New Report DateWise Summary Report
</commit_message>
<xml_diff>
--- a/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
+++ b/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="48">
   <si>
     <t>S.N</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Valid Run ID message in Report Page while click on "0" RunID.</t>
+  </si>
+  <si>
+    <t>Archive logic in Rule service</t>
   </si>
 </sst>
 </file>
@@ -565,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1127,7 @@
       </c>
       <c r="H22" s="14"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1213,16 +1216,26 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="B27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="11">
+        <v>43172</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">

</xml_diff>

<commit_message>
implement utility project and API related db changes
</commit_message>
<xml_diff>
--- a/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
+++ b/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
   <si>
     <t>S.N</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Data must be saved / Modify the config file value as well as config table value: Configuration page</t>
   </si>
   <si>
-    <t>Monthly/Weekly document processing report with graphical format</t>
-  </si>
-  <si>
     <t>Drildown report with service log and its result</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>ApplyRule: Choose one document to locate the folder</t>
   </si>
   <si>
-    <t>New Page for Validation rule/ we can integrate it in Rule builder page (Need to decide)</t>
-  </si>
-  <si>
     <t>Stop showing '0' with Running status in summary report</t>
   </si>
   <si>
@@ -168,6 +162,24 @@
   </si>
   <si>
     <t>Archive logic in Rule service</t>
+  </si>
+  <si>
+    <t>Date wise summary report</t>
+  </si>
+  <si>
+    <t>Monthly/Weekly/Daily document processing report with graphical format</t>
+  </si>
+  <si>
+    <t>DateWiseSummaryReport.aspx</t>
+  </si>
+  <si>
+    <t>Implement Session in every page</t>
+  </si>
+  <si>
+    <t>Date wise summary report showing date and time both. Should show date only</t>
+  </si>
+  <si>
+    <t>New Page for Validation rule/ we can integrate it in Rule builder page (Need to decide) (Ref. 13)</t>
   </si>
 </sst>
 </file>
@@ -194,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,12 +228,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -285,7 +291,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +586,7 @@
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -606,10 +611,10 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -630,7 +635,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="6"/>
       <c r="U2" s="1" t="s">
@@ -640,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="X2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -661,7 +666,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="6"/>
       <c r="U3" t="s">
@@ -671,7 +676,7 @@
         <v>13</v>
       </c>
       <c r="X3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -692,7 +697,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="6"/>
       <c r="U4" t="s">
@@ -702,7 +707,7 @@
         <v>11</v>
       </c>
       <c r="X4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -723,7 +728,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="6"/>
       <c r="W5" t="s">
@@ -735,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7">
         <v>43145</v>
@@ -748,7 +753,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="6"/>
       <c r="W6" t="s">
@@ -773,7 +778,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="6"/>
       <c r="W7" t="s">
@@ -798,7 +803,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="9"/>
       <c r="W8" t="s">
@@ -806,26 +811,28 @@
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="7">
         <v>43166</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9" t="s">
+      <c r="D9" s="7">
+        <v>43173</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="9"/>
+      <c r="F9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -845,38 +852,42 @@
         <v>10</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="11">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7">
         <v>43166</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="9"/>
+      <c r="D11" s="7">
+        <v>43172</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="7">
         <v>43164</v>
@@ -891,7 +902,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="6"/>
     </row>
@@ -900,7 +911,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="11">
         <v>43166</v>
@@ -913,7 +924,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="9"/>
     </row>
@@ -922,7 +933,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="11">
         <v>43166</v>
@@ -935,7 +946,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="9"/>
     </row>
@@ -944,7 +955,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C15" s="11">
         <v>43166</v>
@@ -957,7 +968,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="9"/>
     </row>
@@ -966,7 +977,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="11">
         <v>43166</v>
@@ -979,10 +990,10 @@
         <v>10</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -990,7 +1001,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="7">
         <v>43166</v>
@@ -1005,7 +1016,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H17" s="6"/>
     </row>
@@ -1014,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="7">
         <v>43166</v>
@@ -1029,10 +1040,10 @@
         <v>14</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1040,7 +1051,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="11">
         <v>43166</v>
@@ -1053,10 +1064,10 @@
         <v>10</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1064,7 +1075,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="11">
         <v>43166</v>
@@ -1077,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H20" s="9"/>
     </row>
@@ -1086,7 +1097,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="11">
         <v>43166</v>
@@ -1099,7 +1110,7 @@
         <v>10</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H21" s="9"/>
     </row>
@@ -1108,7 +1119,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="7">
         <v>43167</v>
@@ -1123,16 +1134,16 @@
         <v>15</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="11">
         <v>43167</v>
@@ -1145,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H23" s="9"/>
     </row>
@@ -1154,7 +1165,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" s="11">
         <v>43171</v>
@@ -1167,7 +1178,7 @@
         <v>10</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H24" s="9"/>
     </row>
@@ -1176,7 +1187,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="11">
         <v>43171</v>
@@ -1189,38 +1200,40 @@
         <v>10</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="11">
+      <c r="B26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="7">
         <v>43171</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" s="9"/>
+      <c r="D26" s="7">
+        <v>43173</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="11">
         <v>43172</v>
@@ -1233,33 +1246,319 @@
         <v>10</v>
       </c>
       <c r="G27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="7">
+        <v>43172</v>
+      </c>
+      <c r="D28" s="7">
+        <v>43173</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="11">
+        <v>43173</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="11">
+        <v>43173</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H29"/>

</xml_diff>

<commit_message>
add doctype ,change in db, and solve radio button click problem
</commit_message>
<xml_diff>
--- a/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
+++ b/Lateetud.RuleEngineAppAspNet/QA and SQLScripts/IssueTracker_RuleBuilder.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,26 +973,28 @@
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>15</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="7">
         <v>43166</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="9" t="s">
+      <c r="D16" s="7">
+        <v>43179</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1047,26 +1049,28 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="7">
         <v>43166</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="D19" s="7">
+        <v>43179</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1139,26 +1143,28 @@
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="7">
         <v>43167</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="9" t="s">
+      <c r="D23" s="7">
+        <v>43180</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="9">

</xml_diff>